<commit_message>
JS8_Praktikum 3 – Implementasi Export PDF di Laravel dengan dompdf
</commit_message>
<xml_diff>
--- a/Week 8/PWL_POS/public/template_barang.xlsx
+++ b/Week 8/PWL_POS/public/template_barang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KULIAH\SEMESTER-4\file\laragon\www\PROWEBLNJT\Week 8\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FAB02E-B97F-47CC-A8E3-0570C73E117A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA85ADF-E601-4E4C-B4C6-33F783B7B602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>kategori_id</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>Pasta gigi (75ml)</t>
+  </si>
+  <si>
+    <t>kategori_nama</t>
+  </si>
+  <si>
+    <t>Personal Care</t>
+  </si>
+  <si>
+    <t>Baby Product</t>
   </si>
 </sst>
 </file>
@@ -404,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,9 +426,10 @@
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -435,8 +445,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -452,8 +465,11 @@
       <c r="E2">
         <v>4500</v>
       </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -469,8 +485,11 @@
       <c r="E3">
         <v>7500</v>
       </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -486,8 +505,11 @@
       <c r="E4">
         <v>250000</v>
       </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -503,8 +525,11 @@
       <c r="E5">
         <v>64000</v>
       </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -519,6 +544,9 @@
       </c>
       <c r="E6">
         <v>22000</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>